<commit_message>
Matriz de marco de trabajo
</commit_message>
<xml_diff>
--- a/Documentación/PREGAME/1.ELICITACIÓN/1.1 Especificación RS/Backlog-1Sprint0 V1.0.xlsx
+++ b/Documentación/PREGAME/1.ELICITACIÓN/1.1 Especificación RS/Backlog-1Sprint0 V1.0.xlsx
@@ -1048,11 +1048,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2082600281"/>
-        <c:axId val="1456341701"/>
+        <c:axId val="557120221"/>
+        <c:axId val="793980704"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2082600281"/>
+        <c:axId val="557120221"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1104,10 +1104,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1456341701"/>
+        <c:crossAx val="793980704"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1456341701"/>
+        <c:axId val="793980704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1171,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2082600281"/>
+        <c:crossAx val="557120221"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1264,11 +1264,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1655009203"/>
-        <c:axId val="2009422658"/>
+        <c:axId val="425224300"/>
+        <c:axId val="1754114074"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1655009203"/>
+        <c:axId val="425224300"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,10 +1320,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2009422658"/>
+        <c:crossAx val="1754114074"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2009422658"/>
+        <c:axId val="1754114074"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1387,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1655009203"/>
+        <c:crossAx val="425224300"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1847,11 +1847,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2112489104"/>
-        <c:axId val="1944266842"/>
+        <c:axId val="193799943"/>
+        <c:axId val="1400018057"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2112489104"/>
+        <c:axId val="193799943"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,10 +1903,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1944266842"/>
+        <c:crossAx val="1400018057"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1944266842"/>
+        <c:axId val="1400018057"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1970,7 +1970,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112489104"/>
+        <c:crossAx val="193799943"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>